<commit_message>
Blake Wingrove Project upload
</commit_message>
<xml_diff>
--- a/Project/Project data.xlsx
+++ b/Project/Project data.xlsx
@@ -8,38 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GW/Desktop/Evolution/tasks/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A38341-A693-824A-A8F2-7E094B666692}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF6E1E-C1C1-1046-B5FB-9CF852466064}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{BEE33FC7-A5E5-DA46-8364-4F69DCA36168}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{BEE33FC7-A5E5-DA46-8364-4F69DCA36168}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet5!$B$5:$B$13</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet5!$C$4</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet5!$C$5:$C$13</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet5!$D$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet5!$D$5:$D$13</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Sheet5!$B$5:$B$13</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">Sheet5!$C$4</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">Sheet5!$C$5:$C$13</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">Sheet5!$D$4</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">Sheet5!$D$5:$D$13</definedName>
-    <definedName name="_xlchart.v5.0" hidden="1">Sheet5!$B$4</definedName>
-    <definedName name="_xlchart.v5.1" hidden="1">Sheet5!$B$5:$B$13</definedName>
-    <definedName name="_xlchart.v5.10" hidden="1">Sheet5!$C$4</definedName>
-    <definedName name="_xlchart.v5.11" hidden="1">Sheet5!$C$5:$C$13</definedName>
-    <definedName name="_xlchart.v5.2" hidden="1">Sheet5!$C$4</definedName>
-    <definedName name="_xlchart.v5.3" hidden="1">Sheet5!$C$5:$C$13</definedName>
-    <definedName name="_xlchart.v5.4" hidden="1">Sheet5!$B$4</definedName>
-    <definedName name="_xlchart.v5.5" hidden="1">Sheet5!$B$5:$B$13</definedName>
-    <definedName name="_xlchart.v5.6" hidden="1">Sheet5!$C$4</definedName>
-    <definedName name="_xlchart.v5.7" hidden="1">Sheet5!$C$5:$C$13</definedName>
-    <definedName name="_xlchart.v5.8" hidden="1">Sheet5!$B$4</definedName>
-    <definedName name="_xlchart.v5.9" hidden="1">Sheet5!$B$5:$B$13</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet5!$G$5:$G$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet5!$H$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet5!$H$5:$H$12</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet5!$I$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet5!$I$5:$I$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="73">
   <si>
     <t>ID_Pup</t>
   </si>
@@ -160,12 +147,129 @@
   <si>
     <t xml:space="preserve">Avg Weight </t>
   </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>Anova: Single Factor</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Source of Variation</t>
+  </si>
+  <si>
+    <t>F crit</t>
+  </si>
+  <si>
+    <t>Between Groups</t>
+  </si>
+  <si>
+    <t>Within Groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg Weight FWB </t>
+  </si>
+  <si>
+    <t>Avg Aggressivness FWB</t>
+  </si>
+  <si>
+    <t>Avg Weight SSB</t>
+  </si>
+  <si>
+    <t>Avg Aggressivness SBB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,6 +290,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -203,14 +315,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,7 +403,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>FWB RESULTS</a:t>
+              <a:t>Fresh Water Beach RESULTS</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -312,7 +452,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Weight </c:v>
+                  <c:v>Avg Weight FWB </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -428,7 +568,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Aggressivness</c:v>
+                  <c:v>Avg Aggressivness FWB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -894,7 +1034,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>SSB</a:t>
+              <a:t>Special Study Beach</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -948,7 +1088,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Weight </c:v>
+                  <c:v>Avg Weight SSB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1058,7 +1198,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg Aggressivness</c:v>
+                  <c:v>Avg Aggressivness SBB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2950,13 +3090,13 @@
       <selection sqref="A1:L56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2989,7 +3129,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3055,7 +3195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3088,7 +3228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3121,7 +3261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3154,7 +3294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3223,7 +3363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -3259,7 +3399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3295,7 +3435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3328,7 +3468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3361,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -3394,7 +3534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -3427,7 +3567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3460,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3493,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -3526,7 +3666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3559,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -3592,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -3625,7 +3765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -3658,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3691,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -3724,7 +3864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3757,7 +3897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3790,7 +3930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3823,7 +3963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -3856,7 +3996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3889,7 +4029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -3922,7 +4062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -3955,7 +4095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3988,7 +4128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -4021,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -4054,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -4087,7 +4227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -4120,7 +4260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -4153,7 +4293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -4186,7 +4326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -4219,7 +4359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -4252,7 +4392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -4285,7 +4425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -4318,7 +4458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -4351,7 +4491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -4384,7 +4524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -4417,7 +4557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -4450,7 +4590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -4483,7 +4623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -4516,7 +4656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -4549,7 +4689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -4582,7 +4722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -4615,7 +4755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -4648,7 +4788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H52" s="2" t="s">
         <v>23</v>
       </c>
@@ -4665,7 +4805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H53" s="2" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H54" s="2" t="s">
         <v>23</v>
       </c>
@@ -4699,7 +4839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H55" s="2" t="s">
         <v>23</v>
       </c>
@@ -4716,7 +4856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H56" s="2" t="s">
         <v>23</v>
       </c>
@@ -4746,7 +4886,7 @@
       <selection activeCell="Q61" sqref="Q61:X70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
@@ -4756,7 +4896,7 @@
     <col min="24" max="24" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4789,7 +4929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4822,7 +4962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4855,7 +4995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4888,7 +5028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4921,7 +5061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4954,7 +5094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4987,7 +5127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -5020,7 +5160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -5053,7 +5193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -5086,7 +5226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -5119,7 +5259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5152,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -5185,7 +5325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -5218,7 +5358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -5251,7 +5391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5284,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -5317,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -5350,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -5383,7 +5523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -5416,7 +5556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -5449,7 +5589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -5482,7 +5622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -5515,7 +5655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -5548,7 +5688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -5581,7 +5721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -5614,7 +5754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -5647,7 +5787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -5680,7 +5820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -5713,7 +5853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -5746,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -5779,7 +5919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -5812,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -5845,7 +5985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -5878,7 +6018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -5911,7 +6051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -5944,7 +6084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -5977,7 +6117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -6010,7 +6150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -6043,7 +6183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -6076,7 +6216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -6109,7 +6249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -6142,7 +6282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -6175,7 +6315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -6208,7 +6348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -6241,7 +6381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -6274,7 +6414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -6307,7 +6447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -6340,7 +6480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -6373,7 +6513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -6406,7 +6546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -6439,7 +6579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H52" s="2" t="s">
         <v>23</v>
       </c>
@@ -6456,7 +6596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H53" s="2" t="s">
         <v>23</v>
       </c>
@@ -6473,7 +6613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H54" s="2" t="s">
         <v>23</v>
       </c>
@@ -6490,7 +6630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H55" s="2" t="s">
         <v>23</v>
       </c>
@@ -6507,7 +6647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H56" s="2" t="s">
         <v>23</v>
       </c>
@@ -6524,7 +6664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="Q61" t="s">
         <v>3</v>
       </c>
@@ -6544,7 +6684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -6600,7 +6740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -6658,7 +6798,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
@@ -6708,7 +6848,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -6762,7 +6902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>4</v>
       </c>
@@ -6816,7 +6956,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -6874,7 +7014,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -6924,7 +7064,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -6974,7 +7114,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -7012,7 +7152,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -7038,7 +7178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -7064,7 +7204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -7098,7 +7238,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -7132,7 +7272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -7158,7 +7298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -7184,7 +7324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -7210,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:24">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -7236,7 +7376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:24">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -7262,7 +7402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:24">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>6</v>
       </c>
@@ -7296,7 +7436,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>6</v>
       </c>
@@ -7330,7 +7470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -7356,7 +7496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>6</v>
       </c>
@@ -7382,7 +7522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -7408,7 +7548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
@@ -7442,7 +7582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
@@ -7476,7 +7616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
@@ -7502,7 +7642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
@@ -7528,7 +7668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -7554,7 +7694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -7588,7 +7728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -7614,7 +7754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
@@ -7640,7 +7780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -7674,7 +7814,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
@@ -7700,7 +7840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>9</v>
       </c>
@@ -7726,7 +7866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -7752,7 +7892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -7786,7 +7926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>9</v>
       </c>
@@ -7812,7 +7952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -7846,7 +7986,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -7872,7 +8012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -7898,7 +8038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>10</v>
       </c>
@@ -7924,7 +8064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>10</v>
       </c>
@@ -7950,7 +8090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>10</v>
       </c>
@@ -7984,7 +8124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -8010,7 +8150,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>10</v>
       </c>
@@ -8036,7 +8176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>10</v>
       </c>
@@ -8070,7 +8210,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>11</v>
       </c>
@@ -8096,7 +8236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>11</v>
       </c>
@@ -8122,7 +8262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>11</v>
       </c>
@@ -8156,7 +8296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>11</v>
       </c>
@@ -8182,7 +8322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>11</v>
       </c>
@@ -8208,7 +8348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="8:13">
+    <row r="113" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H113" s="2" t="s">
         <v>23</v>
       </c>
@@ -8222,7 +8362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="8:13">
+    <row r="114" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H114" s="2" t="s">
         <v>23</v>
       </c>
@@ -8244,7 +8384,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="115" spans="8:13">
+    <row r="115" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H115" s="2" t="s">
         <v>23</v>
       </c>
@@ -8258,7 +8398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="8:13">
+    <row r="116" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H116" s="2" t="s">
         <v>23</v>
       </c>
@@ -8272,7 +8412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="8:13">
+    <row r="117" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H117" s="2" t="s">
         <v>23</v>
       </c>
@@ -8292,40 +8432,830 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6294F0DE-49E8-6449-B216-9C8C202FBF4E}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.5344821364183221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.28567115415029393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.18362417617176449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.51659257481273546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.74707217382868696</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.74707217382868696</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.7994082706731289</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.13821539625356632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.8680752184615621</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.26686788835165171</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.6151473922902491</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3.2445763438874229</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.88504743838081956</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3.6659914521907715</v>
+      </c>
+      <c r="E17" s="3">
+        <v>8.0065824610432365E-3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1.1517717072820659</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5.3373809804927799</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.1517717072820659</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5.3373809804927799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4">
+        <v>-0.20361876608199114</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.12169834736038897</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-1.673143230770495</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.13821539625356641</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-0.49138962962912969</v>
+      </c>
+      <c r="G18" s="4">
+        <v>8.4152097465147402E-2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>-0.49138962962912969</v>
+      </c>
+      <c r="I18" s="4">
+        <v>8.4152097465147402E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBE30A7-1593-884A-994F-A174F1F597F6}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.40390579425154194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.16313989062996892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.3663205734963721E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.6788012899008069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.53894428154543306</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.53894428154543306</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.1696570703037346</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.32101189434799421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2.7646271470259958</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.46077119117099929</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.3035714285714288</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3">
+        <v>-0.15973814267276554</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2.3559651411153637</v>
+      </c>
+      <c r="D17" s="3">
+        <v>-6.7801573072996377E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.94814657572736571</v>
+      </c>
+      <c r="F17" s="3">
+        <v>-5.9245771673523802</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5.6051008820068482</v>
+      </c>
+      <c r="H17" s="3">
+        <v>-5.9245771673523802</v>
+      </c>
+      <c r="I17" s="3">
+        <v>5.6051008820068482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.30923786933591707</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.28593241813115394</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.0815068517137263</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.32101189434799382</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-0.39041355321574228</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.0088892918875765</v>
+      </c>
+      <c r="H18" s="4">
+        <v>-0.39041355321574228</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.0088892918875765</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECEB860-4673-494C-8425-284C9E07FECC}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>65.57380952380953</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8.1967261904761912</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.80511975623582133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.375</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.47193877551020436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3">
+        <v>135.56998334750566</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>135.56998334750566</v>
+      </c>
+      <c r="E11" s="3">
+        <v>212.31600584845606</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7.4663592147263992E-10</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4.6001099366694227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3">
+        <v>8.9394097222222264</v>
+      </c>
+      <c r="C12" s="3">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.63852926587301617</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>144.50939306972788</v>
+      </c>
+      <c r="C14" s="4">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB116BB-783C-5847-AFCA-4099E81CACE6}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>64.201428571428579</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.1334920634920644</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.2523556689342215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16.12857142857143</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.7920634920634921</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.3268934240362813</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3">
+        <v>128.38886632653063</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>128.38886632653063</v>
+      </c>
+      <c r="E11" s="3">
+        <v>99.55522843950304</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.8333511402164309E-8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4.4939984776663584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3">
+        <v>20.633992743764171</v>
+      </c>
+      <c r="C12" s="3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.2896245464852607</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4">
+        <v>149.0228590702948</v>
+      </c>
+      <c r="C14" s="4">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5352CFC-66ED-F34C-8BF6-B6A642EE4A78}">
   <dimension ref="B4:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -8345,7 +9275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -8365,7 +9295,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -8385,7 +9315,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -8405,7 +9335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -8425,7 +9355,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -8445,7 +9375,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -8465,7 +9395,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -8485,7 +9415,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Blake Wingrove Task 05 upload
</commit_message>
<xml_diff>
--- a/Project/Project data.xlsx
+++ b/Project/Project data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GW/Desktop/Evolution/tasks/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF6E1E-C1C1-1046-B5FB-9CF852466064}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37809C7-3466-8744-984E-E6D8ADD3A190}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{BEE33FC7-A5E5-DA46-8364-4F69DCA36168}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BEE33FC7-A5E5-DA46-8364-4F69DCA36168}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,6 @@
     <sheet name="Sheet9" sheetId="9" r:id="rId6"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet5!$G$5:$G$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet5!$H$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet5!$H$5:$H$12</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet5!$I$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet5!$I$5:$I$12</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="75">
   <si>
     <t>ID_Pup</t>
   </si>
@@ -264,12 +257,18 @@
   <si>
     <t>Avg Aggressivness SBB</t>
   </si>
+  <si>
+    <t>SUMMARY FWB</t>
+  </si>
+  <si>
+    <t>SUMMARY SSB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -481,6 +480,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet5!$B$5:$B$13</c:f>
@@ -559,6 +573,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1385387680"/>
+        <c:axId val="1386103104"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -597,6 +627,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet5!$B$5:$B$13</c:f>
@@ -685,8 +729,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1385387680"/>
-        <c:axId val="1386103104"/>
+        <c:axId val="1487661119"/>
+        <c:axId val="1849834847"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1385387680"/>
@@ -916,6 +960,120 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="1849834847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Aggressivness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1487661119"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1487661119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1849834847"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1117,6 +1275,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet5!$G$5:$G$12</c:f>
@@ -1189,6 +1361,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1385437808"/>
+        <c:axId val="1385931024"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1227,6 +1415,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet5!$G$5:$G$12</c:f>
@@ -1309,8 +1511,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1385437808"/>
-        <c:axId val="1385931024"/>
+        <c:axId val="1480360863"/>
+        <c:axId val="1933973391"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1385437808"/>
@@ -1380,7 +1582,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1506,7 +1708,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1541,6 +1743,121 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="1933973391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Aggressivness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1480360863"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1480360863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1933973391"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2716,14 +3033,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>140855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3086,17 +3403,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8C31AF-F030-6149-91AA-CC836F9D42AF}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3129,7 +3446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3162,7 +3479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3195,7 +3512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3228,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3261,7 +3578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3294,7 +3611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3327,7 +3644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3363,7 +3680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -3399,7 +3716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -3435,7 +3752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -3468,7 +3785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -3501,7 +3818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -3534,7 +3851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -3567,7 +3884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -3600,7 +3917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -3633,7 +3950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -3666,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3699,7 +4016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -3732,7 +4049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -3765,7 +4082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -3798,7 +4115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3831,7 +4148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -3864,7 +4181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3897,7 +4214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3930,7 +4247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3963,7 +4280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -3996,7 +4313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -4029,7 +4346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -4062,7 +4379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -4095,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -4128,7 +4445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -4161,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -4194,7 +4511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -4227,7 +4544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -4260,7 +4577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -4293,7 +4610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -4326,7 +4643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -4359,7 +4676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -4392,7 +4709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -4425,7 +4742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -4458,7 +4775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -4491,7 +4808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -4524,7 +4841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -4557,7 +4874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -4590,7 +4907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -4623,7 +4940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -4656,7 +4973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -4689,7 +5006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -4722,7 +5039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -4755,7 +5072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -4788,7 +5105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="H52" s="2" t="s">
         <v>23</v>
       </c>
@@ -4805,7 +5122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="H53" s="2" t="s">
         <v>23</v>
       </c>
@@ -4822,7 +5139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="H54" s="2" t="s">
         <v>23</v>
       </c>
@@ -4839,7 +5156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="H55" s="2" t="s">
         <v>23</v>
       </c>
@@ -4856,7 +5173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="H56" s="2" t="s">
         <v>23</v>
       </c>
@@ -4886,7 +5203,7 @@
       <selection activeCell="Q61" sqref="Q61:X70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
@@ -4896,7 +5213,7 @@
     <col min="24" max="24" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4929,7 +5246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4962,7 +5279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4995,7 +5312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -5028,7 +5345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5061,7 +5378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -5094,7 +5411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5127,7 +5444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -5160,7 +5477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -5193,7 +5510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -5226,7 +5543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -5259,7 +5576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -5292,7 +5609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -5325,7 +5642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -5358,7 +5675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -5391,7 +5708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5424,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -5457,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -5490,7 +5807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -5523,7 +5840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -5556,7 +5873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -5589,7 +5906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -5622,7 +5939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -5655,7 +5972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -5688,7 +6005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -5721,7 +6038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -5754,7 +6071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -5787,7 +6104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -5820,7 +6137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -5853,7 +6170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -5886,7 +6203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -5919,7 +6236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -5952,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -5985,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -6018,7 +6335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -6051,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -6084,7 +6401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -6117,7 +6434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -6150,7 +6467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -6183,7 +6500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -6216,7 +6533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -6249,7 +6566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -6282,7 +6599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -6315,7 +6632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -6348,7 +6665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -6381,7 +6698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -6414,7 +6731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -6447,7 +6764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>11</v>
       </c>
@@ -6480,7 +6797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24">
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
@@ -6513,7 +6830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -6546,7 +6863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:24">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -6579,7 +6896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:24">
       <c r="H52" s="2" t="s">
         <v>23</v>
       </c>
@@ -6596,7 +6913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:24">
       <c r="H53" s="2" t="s">
         <v>23</v>
       </c>
@@ -6613,7 +6930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:24">
       <c r="H54" s="2" t="s">
         <v>23</v>
       </c>
@@ -6630,7 +6947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24">
       <c r="H55" s="2" t="s">
         <v>23</v>
       </c>
@@ -6647,7 +6964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:24">
       <c r="H56" s="2" t="s">
         <v>23</v>
       </c>
@@ -6664,7 +6981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:24">
       <c r="Q61" t="s">
         <v>3</v>
       </c>
@@ -6684,7 +7001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:24">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -6740,7 +7057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -6798,7 +7115,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24">
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
@@ -6848,7 +7165,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:24">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -6902,7 +7219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:24">
       <c r="A66" s="1" t="s">
         <v>4</v>
       </c>
@@ -6956,7 +7273,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:24">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -7014,7 +7331,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:24">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -7064,7 +7381,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:24">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -7114,7 +7431,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:24">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -7152,7 +7469,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:24">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
@@ -7178,7 +7495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:24">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -7204,7 +7521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:24">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -7238,7 +7555,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:24">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -7272,7 +7589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:24">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
@@ -7298,7 +7615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:24">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
@@ -7324,7 +7641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:24">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -7350,7 +7667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:24">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -7376,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:24">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -7402,7 +7719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:24">
       <c r="A80" s="1" t="s">
         <v>6</v>
       </c>
@@ -7436,7 +7753,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
         <v>6</v>
       </c>
@@ -7470,7 +7787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -7496,7 +7813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83" s="1" t="s">
         <v>6</v>
       </c>
@@ -7522,7 +7839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -7548,7 +7865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
@@ -7582,7 +7899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
@@ -7616,7 +7933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
@@ -7642,7 +7959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
@@ -7668,7 +7985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -7694,7 +8011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -7728,7 +8045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -7754,7 +8071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
@@ -7780,7 +8097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -7814,7 +8131,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="A94" s="1" t="s">
         <v>9</v>
       </c>
@@ -7840,7 +8157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="A95" s="1" t="s">
         <v>9</v>
       </c>
@@ -7866,7 +8183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
@@ -7892,7 +8209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -7926,7 +8243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13">
       <c r="A98" s="1" t="s">
         <v>9</v>
       </c>
@@ -7952,7 +8269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13">
       <c r="A99" s="1" t="s">
         <v>9</v>
       </c>
@@ -7986,7 +8303,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
         <v>9</v>
       </c>
@@ -8012,7 +8329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -8038,7 +8355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
         <v>10</v>
       </c>
@@ -8064,7 +8381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
         <v>10</v>
       </c>
@@ -8090,7 +8407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13">
       <c r="A104" s="1" t="s">
         <v>10</v>
       </c>
@@ -8124,7 +8441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -8150,7 +8467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13">
       <c r="A106" s="1" t="s">
         <v>10</v>
       </c>
@@ -8176,7 +8493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13">
       <c r="A107" s="1" t="s">
         <v>10</v>
       </c>
@@ -8210,7 +8527,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
         <v>11</v>
       </c>
@@ -8236,7 +8553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13">
       <c r="A109" s="1" t="s">
         <v>11</v>
       </c>
@@ -8262,7 +8579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13">
       <c r="A110" s="1" t="s">
         <v>11</v>
       </c>
@@ -8296,7 +8613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
         <v>11</v>
       </c>
@@ -8322,7 +8639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13">
       <c r="A112" s="1" t="s">
         <v>11</v>
       </c>
@@ -8348,7 +8665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="8:13">
       <c r="H113" s="2" t="s">
         <v>23</v>
       </c>
@@ -8362,7 +8679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="8:13">
       <c r="H114" s="2" t="s">
         <v>23</v>
       </c>
@@ -8384,7 +8701,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="115" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="8:13">
       <c r="H115" s="2" t="s">
         <v>23</v>
       </c>
@@ -8398,7 +8715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="8:13">
       <c r="H116" s="2" t="s">
         <v>23</v>
       </c>
@@ -8412,7 +8729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="8:13">
       <c r="H117" s="2" t="s">
         <v>23</v>
       </c>
@@ -8439,21 +8756,21 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17" thickBot="1"/>
+    <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -8461,7 +8778,7 @@
         <v>0.5344821364183221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -8469,7 +8786,7 @@
         <v>0.28567115415029393</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -8477,7 +8794,7 @@
         <v>0.18362417617176449</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -8485,7 +8802,7 @@
         <v>0.51659257481273546</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -8493,12 +8810,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17" thickBot="1">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>46</v>
@@ -8516,7 +8833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -8536,7 +8853,7 @@
         <v>0.13821539625356632</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -8552,7 +8869,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -8566,8 +8883,8 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17" thickBot="1"/>
+    <row r="16" spans="1:9">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>50</v>
@@ -8594,7 +8911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -8623,7 +8940,7 @@
         <v>5.3373809804927799</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="17" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -8662,24 +8979,24 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I21"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17" thickBot="1"/>
+    <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -8687,7 +9004,7 @@
         <v>0.40390579425154194</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -8695,7 +9012,7 @@
         <v>0.16313989062996892</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -8703,7 +9020,7 @@
         <v>2.3663205734963721E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -8711,7 +9028,7 @@
         <v>0.6788012899008069</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -8719,12 +9036,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17" thickBot="1">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>46</v>
@@ -8742,7 +9059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -8762,7 +9079,7 @@
         <v>0.32101189434799421</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -8778,7 +9095,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -8792,8 +9109,8 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17" thickBot="1"/>
+    <row r="16" spans="1:9">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>50</v>
@@ -8820,7 +9137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -8849,7 +9166,7 @@
         <v>5.6051008820068482</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="17" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -8885,25 +9202,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECEB860-4673-494C-8425-284C9E07FECC}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A3:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="17" thickBot="1">
       <c r="A3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -8920,7 +9238,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -8937,7 +9255,7 @@
         <v>0.80511975623582133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -8954,12 +9272,12 @@
         <v>0.47193877551020436</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17" thickBot="1">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
@@ -8982,7 +9300,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -9005,7 +9323,7 @@
         <v>4.6001099366694227</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -9022,7 +9340,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -9031,7 +9349,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="17" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -9046,8 +9364,157 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
+    <row r="16" spans="1:7" ht="17" thickBot="1">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3">
+        <v>64.201428571428579</v>
+      </c>
+      <c r="D18" s="3">
+        <v>7.1334920634920644</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2.2523556689342215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1">
+      <c r="A19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4">
+        <v>16.12857142857143</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.7920634920634921</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.3268934240362813</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" thickBot="1">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="3">
+        <v>128.38886632653063</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>128.38886632653063</v>
+      </c>
+      <c r="E24" s="3">
+        <v>99.55522843950304</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2.8333511402164309E-8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4.4939984776663584</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="3">
+        <v>20.633992743764171</v>
+      </c>
+      <c r="C25" s="3">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.2896245464852607</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="17" thickBot="1">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="4">
+        <v>149.0228590702948</v>
+      </c>
+      <c r="C27" s="4">
+        <v>17</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9055,23 +9522,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB116BB-783C-5847-AFCA-4099E81CACE6}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G14"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="17" thickBot="1">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -9088,7 +9558,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -9105,7 +9575,7 @@
         <v>2.2523556689342215</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17" thickBot="1">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -9122,12 +9592,12 @@
         <v>0.3268934240362813</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17" thickBot="1">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
@@ -9150,7 +9620,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -9173,7 +9643,7 @@
         <v>4.4939984776663584</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -9190,7 +9660,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -9199,7 +9669,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="17" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -9221,13 +9691,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5352CFC-66ED-F34C-8BF6-B6A642EE4A78}">
-  <dimension ref="B4:I13"/>
+  <dimension ref="B4:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
@@ -9235,7 +9705,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -9255,7 +9725,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -9275,7 +9745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -9295,7 +9765,7 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -9315,7 +9785,7 @@
         <v>1.1428571428571428</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -9335,7 +9805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -9355,7 +9825,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -9375,7 +9845,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -9395,7 +9865,7 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -9415,7 +9885,7 @@
         <v>2.2857142857142856</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -9424,6 +9894,26 @@
       </c>
       <c r="D13">
         <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="H14">
+        <f>AVERAGE(H5:H12)</f>
+        <v>8.1967261904761912</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(I5:I12)</f>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="C15">
+        <f>AVERAGE(C5:C13)</f>
+        <v>7.1334920634920644</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D5:D13)</f>
+        <v>1.7920634920634921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>